<commit_message>
Case1 scenarios & price
Scenarios: Random1 e Random2 hanno diverso ordine di profili PV
Price: 3 scenarios of price for Induction Stove
</commit_message>
<xml_diff>
--- a/tesi_camilla/profiles generation/1Data_input_DPT.xlsx
+++ b/tesi_camilla/profiles generation/1Data_input_DPT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cami/Documents/GitHub/pyesm_thesis/tesi_camilla/profiles generation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654F3705-BBA5-134B-9718-35FA5113EB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0DBB80-94E5-434A-9553-8EA090559110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,7 +345,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -358,6 +358,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -388,11 +398,121 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -704,15 +824,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -731,8 +851,9 @@
       <c r="I1" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -755,7 +876,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -778,7 +899,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -801,7 +922,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -809,7 +930,7 @@
         <v>6.5453124999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -836,7 +957,7 @@
         <v>63.65</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -863,7 +984,7 @@
         <v>70.350000000000009</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -890,7 +1011,7 @@
         <v>63.649999999999991</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -898,7 +1019,7 @@
         <v>8.5734375000000007</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -925,7 +1046,7 @@
         <v>59.350000000000009</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -933,7 +1054,7 @@
         <v>6.5453124999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -941,7 +1062,7 @@
         <v>6.4223958333333337</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -949,7 +1070,7 @@
         <v>6.4223958333333337</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -957,7 +1078,7 @@
         <v>13.797395833333329</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -965,7 +1086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1310,38 +1431,56 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J8">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="between">
+      <formula>$F$6</formula>
+      <formula>$F$7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="between">
+      <formula>$G$6</formula>
+      <formula>$G$7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="between">
+      <formula>$I$6</formula>
+      <formula>$I$7</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F8:I8">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="between">
       <formula>$F$6</formula>
       <formula>$F$7</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="between">
+      <formula>$G$6</formula>
+      <formula>$G$7</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G8:I8">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="between">
       <formula>$G$6</formula>
       <formula>$G$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
       <formula>$H$6</formula>
       <formula>$H$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="between">
       <formula>$H$6</formula>
       <formula>$H$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="between">
       <formula>$I$6</formula>
       <formula>$I$7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
-      <formula>$G$6</formula>
-      <formula>$G$7</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>